<commit_message>
update dataset Arion spp.
</commit_message>
<xml_diff>
--- a/data/raw/NorthernSpain_ES_TOTAL_v1.xlsx
+++ b/data/raw/NorthernSpain_ES_TOTAL_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WARD\OneDrive - UGent\School\1ste master\sem_2\Project\landsnails-Spain\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="490" documentId="13_ncr:1_{2E796F1C-C6A4-4BA0-8FBB-0E686A07A5DC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{E7A7A766-49A8-4989-92FA-073B685F3F7B}"/>
+  <xr:revisionPtr revIDLastSave="492" documentId="13_ncr:1_{2E796F1C-C6A4-4BA0-8FBB-0E686A07A5DC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{4444B6B0-31D2-4F0A-9877-9292DED185D9}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,9 +24,9 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId6"/>
-    <pivotCache cacheId="4" r:id="rId7"/>
-    <pivotCache cacheId="5" r:id="rId8"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="1" r:id="rId7"/>
+    <pivotCache cacheId="2" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -4369,7 +4369,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ACAB314E-E09E-4027-984E-A243AF174D67}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ACAB314E-E09E-4027-984E-A243AF174D67}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B80" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -4709,7 +4709,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{51FFF06F-9776-4B31-8FF8-3759F2D892B5}" name="PivotTable4" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{51FFF06F-9776-4B31-8FF8-3759F2D892B5}" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B57" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -4957,7 +4957,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FB2ADF2B-95E8-4768-8AF2-A37328AA3575}" name="PivotTable5" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FB2ADF2B-95E8-4768-8AF2-A37328AA3575}" name="PivotTable5" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B41" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -5406,7 +5406,7 @@
   <dimension ref="A1:AG223"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AF201" sqref="AF201"/>
+      <selection activeCell="D222" sqref="D222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>